<commit_message>
Update deprecated full test files
This is the last modification that will be done for the full test files,
because the application has moved to unit tests instead. These files are
the last remains of the old testing code and will be removed soon.
</commit_message>
<xml_diff>
--- a/tests/local.xlsx
+++ b/tests/local.xlsx
@@ -64,7 +64,7 @@
     <t xml:space="preserve">financial</t>
   </si>
   <si>
-    <t xml:space="preserve">file:///./html/http___catalogos_munimadrid_es_cgi_bin_hemeroteca_TITN_19245.html</t>
+    <t xml:space="preserve">file:///./html/http___catalogos_madrid_es_cgi_bin_hemeroteca_TITN_19245.html</t>
   </si>
   <si>
     <t xml:space="preserve">mill</t>
@@ -73,40 +73,40 @@
     <t xml:space="preserve">move</t>
   </si>
   <si>
-    <t xml:space="preserve">file:///./html/http___catalogos_munimadrid_es_cgi_bin_hemeroteca_TITN_339474.html</t>
+    <t xml:space="preserve">file:///./html/http___catalogos_madrid_es_cgi_bin_hemeroteca_TITN_339474.html</t>
   </si>
   <si>
     <t xml:space="preserve">document</t>
   </si>
   <si>
-    <t xml:space="preserve">file:///./html/http___catalogos_munimadrid_es_cgi_bin_hemeroteca_TITN_52686.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">file:///./html/http___catalogos_munimadrid_es_cgi_bin_historica_TITN_553774.html</t>
+    <t xml:space="preserve">file:///./html/http___catalogos_madrid_es_cgi_bin_hemeroteca_TITN_52686.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file:///./html/http___catalogos_madrid_es_cgi_bin_historica_TITN_553774.html</t>
   </si>
   <si>
     <t xml:space="preserve">hate</t>
   </si>
   <si>
-    <t xml:space="preserve">file:///./html/http___catalogos_munimadrid_es_cgi_bin_historica_TITN_571997.html</t>
+    <t xml:space="preserve">file:///./html/http___catalogos_madrid_es_cgi_bin_historica_TITN_571997.html</t>
   </si>
   <si>
     <t xml:space="preserve">pursuit</t>
   </si>
   <si>
-    <t xml:space="preserve">file:///./html/http___catalogos_munimadrid_es_cgi_bin_historica_TITN_579528.html</t>
+    <t xml:space="preserve">file:///./html/http___catalogos_madrid_es_cgi_bin_historica_TITN_579528.html</t>
   </si>
   <si>
     <t xml:space="preserve">receipt</t>
   </si>
   <si>
-    <t xml:space="preserve">file:///./html/http___catalogos_munimadrid_es_cgi_bin_opacmusical_TITN_334532.html</t>
+    <t xml:space="preserve">file:///./html/http___catalogos_madrid_es_cgi_bin_opacmusical_TITN_334532.html</t>
   </si>
   <si>
     <t xml:space="preserve">definite</t>
   </si>
   <si>
-    <t xml:space="preserve">file:///./html/http___catalogos_munimadrid_es_cgi_bin_opacmusical_TITN_85931.html</t>
+    <t xml:space="preserve">file:///./html/http___catalogos_madrid_es_cgi_bin_opacmusical_TITN_85931.html</t>
   </si>
   <si>
     <t xml:space="preserve">haunt</t>
@@ -310,17 +310,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -336,14 +340,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -625,22 +629,22 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0"/>
+      <c r="B31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0"/>
+      <c r="B32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0"/>
+      <c r="B33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0"/>
+      <c r="B34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0"/>
+      <c r="B35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0"/>
+      <c r="B36" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>